<commit_message>
cambiar tipo de datos
</commit_message>
<xml_diff>
--- a/Archivos Excel/AGUA_CALIENTE_FRIA.xlsx
+++ b/Archivos Excel/AGUA_CALIENTE_FRIA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manee\OneDrive\Escritorio\P_F\PROYECTOS\ANALISIS_GASTO_COMUN\GASTO-COMUN\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1031FD8-0E36-4A91-8225-33CEBC7B560C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABAC8297-875E-4159-A983-4CC043090B12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2616" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{20A801C2-05CB-4726-92C8-0F60FE6665C9}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{20A801C2-05CB-4726-92C8-0F60FE6665C9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -100,8 +100,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,46 +439,46 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>2024</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>1029</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -486,33 +486,33 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>2024</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>1033</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>2024</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>1038</v>
       </c>
       <c r="E4" s="1">
@@ -520,16 +520,16 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>2024</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1039</v>
       </c>
       <c r="E5" s="1">
@@ -537,16 +537,16 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>22</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>2024</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>1040</v>
       </c>
       <c r="E6" s="1">
@@ -554,16 +554,16 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>25</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="1">
         <v>2024</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>1041</v>
       </c>
       <c r="E7" s="1">

</xml_diff>

<commit_message>
Agregar fotos y datos de m3 agua caliente y fria
</commit_message>
<xml_diff>
--- a/Archivos Excel/AGUA_CALIENTE_FRIA.xlsx
+++ b/Archivos Excel/AGUA_CALIENTE_FRIA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manee\OneDrive\Escritorio\P_F\PROYECTOS\ANALISIS_GASTO_COMUN\GASTO-COMUN\Archivos Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC085D72-DE23-4FF1-87D1-0EF47430EA07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69AF7585-438B-40DC-B5F7-F0A33B5583DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{20A801C2-05CB-4726-92C8-0F60FE6665C9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
   <si>
     <t>NaN</t>
   </si>
@@ -63,6 +63,9 @@
   </si>
   <si>
     <t>ANIO</t>
+  </si>
+  <si>
+    <t>Mayo</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272394B7-4C69-409D-A3ED-53DA787BD028}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -587,6 +590,23 @@
         <v>120</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2024</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1042</v>
+      </c>
+      <c r="E9" s="1">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>